<commit_message>
updating time log and project details
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hornb\Documents\EnterpriseJava\myCookbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hornb\Documents\GitHub\my-cookbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Week 2 Exercise Step 4</t>
+  </si>
+  <si>
+    <t>Week 3 Work</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,6 +586,61 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>42738</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>42739</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>42740</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>42741</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>42742</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>